<commit_message>
replace del to ref for insertion variants of NUDT15
</commit_message>
<xml_diff>
--- a/definition/xlsx/NUDT15_allele_definition_table.xlsx
+++ b/definition/xlsx/NUDT15_allele_definition_table.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavita/Dropbox (Personal)/PhamacoProject/allele_definition_table_new_1_12_19_edit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Dropbox\PhamacoProject\allele_definition_table_new_1_12_19_edit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,9 +17,6 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="123">
   <si>
     <t>*1</t>
   </si>
@@ -205,9 +202,6 @@
   </si>
   <si>
     <t>GGAGTC</t>
-  </si>
-  <si>
-    <t>ref</t>
   </si>
   <si>
     <t>NUDT15</t>
@@ -410,7 +404,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -430,7 +424,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -438,40 +432,40 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -484,7 +478,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -894,7 +888,7 @@
     <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1198,11 +1192,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EI31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="H16" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="18.83203125" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" style="9" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="15.33203125" style="10" customWidth="1"/>
@@ -1220,7 +1214,7 @@
     <col min="140" max="16384" width="18.83203125" style="9" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
@@ -1243,15 +1237,15 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
     </row>
-    <row r="2" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>53</v>
@@ -1263,10 +1257,10 @@
         <v>39</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>43</v>
@@ -1275,19 +1269,19 @@
         <v>45</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P2" s="13" t="s">
         <v>24</v>
@@ -1296,18 +1290,18 @@
         <v>25</v>
       </c>
       <c r="R2" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="34" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>54</v>
@@ -1319,10 +1313,10 @@
         <v>30</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>44</v>
@@ -1331,19 +1325,19 @@
         <v>46</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P3" s="13" t="s">
         <v>27</v>
@@ -1352,18 +1346,18 @@
         <v>28</v>
       </c>
       <c r="R3" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" s="7" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="7" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>56</v>
@@ -1372,13 +1366,13 @@
         <v>37</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>50</v>
@@ -1387,19 +1381,19 @@
         <v>51</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>33</v>
@@ -1408,18 +1402,18 @@
         <v>35</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>57</v>
@@ -1431,10 +1425,10 @@
         <v>23</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>48</v>
@@ -1443,19 +1437,19 @@
         <v>49</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N5" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>34</v>
@@ -1464,15 +1458,15 @@
         <v>36</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
@@ -1485,7 +1479,7 @@
         <v>32</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="5" t="s">
@@ -1494,16 +1488,16 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P6" s="15" t="s">
         <v>15</v>
@@ -1512,12 +1506,12 @@
         <v>16</v>
       </c>
       <c r="R6" s="30" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" s="12" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="12" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1537,7 +1531,7 @@
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
     </row>
-    <row r="8" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -1554,10 +1548,10 @@
         <v>7</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>6</v>
@@ -1578,7 +1572,7 @@
         <v>8</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="O8" s="5" t="s">
         <v>7</v>
@@ -1593,7 +1587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>1</v>
       </c>
@@ -1619,7 +1613,7 @@
       <c r="Q9" s="18"/>
       <c r="R9" s="18"/>
     </row>
-    <row r="10" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1643,7 +1637,7 @@
       <c r="Q10" s="18"/>
       <c r="R10" s="18"/>
     </row>
-    <row r="11" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>2</v>
       </c>
@@ -1667,7 +1661,7 @@
       </c>
       <c r="R11" s="18"/>
     </row>
-    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>3</v>
       </c>
@@ -1691,7 +1685,7 @@
       <c r="Q12" s="18"/>
       <c r="R12" s="18"/>
     </row>
-    <row r="13" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>4</v>
       </c>
@@ -1715,7 +1709,7 @@
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
     </row>
-    <row r="14" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>41</v>
       </c>
@@ -1739,7 +1733,7 @@
       <c r="Q14" s="18"/>
       <c r="R14" s="18"/>
     </row>
-    <row r="15" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>42</v>
       </c>
@@ -1763,7 +1757,7 @@
       <c r="Q15" s="18"/>
       <c r="R15" s="18"/>
     </row>
-    <row r="16" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>52</v>
       </c>
@@ -1787,9 +1781,9 @@
       <c r="Q16" s="18"/>
       <c r="R16" s="18"/>
     </row>
-    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>6</v>
@@ -1811,9 +1805,9 @@
       <c r="Q17" s="18"/>
       <c r="R17" s="18"/>
     </row>
-    <row r="18" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -1835,9 +1829,9 @@
       <c r="Q18" s="18"/>
       <c r="R18" s="18"/>
     </row>
-    <row r="19" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -1859,9 +1853,9 @@
       <c r="Q19" s="18"/>
       <c r="R19" s="18"/>
     </row>
-    <row r="20" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -1876,16 +1870,16 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O20" s="5"/>
       <c r="P20" s="18"/>
       <c r="Q20" s="18"/>
       <c r="R20" s="18"/>
     </row>
-    <row r="21" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1893,7 +1887,7 @@
       <c r="E21" s="18"/>
       <c r="F21" s="38"/>
       <c r="G21" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="5"/>
@@ -1907,9 +1901,9 @@
       <c r="Q21" s="18"/>
       <c r="R21" s="18"/>
     </row>
-    <row r="22" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -1931,9 +1925,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -1955,9 +1949,9 @@
       <c r="Q23" s="18"/>
       <c r="R23" s="18"/>
     </row>
-    <row r="24" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
@@ -1979,9 +1973,9 @@
       <c r="Q24" s="18"/>
       <c r="R24" s="18"/>
     </row>
-    <row r="25" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -2003,9 +1997,9 @@
       <c r="Q25" s="18"/>
       <c r="R25" s="18"/>
     </row>
-    <row r="26" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="19" t="s">
@@ -2027,12 +2021,12 @@
       <c r="Q26" s="18"/>
       <c r="R26" s="18"/>
     </row>
-    <row r="28" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:18" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>11</v>
       </c>
@@ -2045,7 +2039,7 @@
       <c r="N29" s="28"/>
       <c r="O29" s="28"/>
     </row>
-    <row r="30" spans="1:18" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
@@ -2058,7 +2052,7 @@
       <c r="N30" s="28"/>
       <c r="O30" s="28"/>
     </row>
-    <row r="31" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -2078,22 +2072,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="32">
         <v>43746</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>